<commit_message>
Latest one from BLS
</commit_message>
<xml_diff>
--- a/resources/Average_hour_earning_by_metropolitan.xlsx
+++ b/resources/Average_hour_earning_by_metropolitan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filer6\didd\SA_Share\SA_DUPS\DCES\2018\Apr2018\Autosuppl\State\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophia_CY_Kang\Desktop\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1433,8 +1433,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="#0.0"/>
-    <numFmt numFmtId="166" formatCode="#0.00"/>
+    <numFmt numFmtId="164" formatCode="#0.0"/>
+    <numFmt numFmtId="165" formatCode="#0.00"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1485,10 +1485,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1781,11 +1781,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J509"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="70" customWidth="1"/>
     <col min="2" max="10" width="15" customWidth="1"/>
@@ -4318,7 +4318,7 @@
         <v>799.21</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="17.25">
+    <row r="88" spans="1:10" ht="16.5">
       <c r="A88" s="3" t="s">
         <v>84</v>
       </c>
@@ -6140,7 +6140,7 @@
         <v>763.43</v>
       </c>
     </row>
-    <row r="150" spans="1:10" ht="17.25">
+    <row r="150" spans="1:10" ht="16.5">
       <c r="A150" s="3" t="s">
         <v>139</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>792.42</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="17.25">
+    <row r="259" spans="1:10" ht="16.5">
       <c r="A259" s="3" t="s">
         <v>230</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>863.33</v>
       </c>
     </row>
-    <row r="341" spans="1:10" ht="17.25">
+    <row r="341" spans="1:10" ht="16.5">
       <c r="A341" s="3" t="s">
         <v>297</v>
       </c>
@@ -16528,6 +16528,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:J3"/>
     <mergeCell ref="A508:J508"/>
     <mergeCell ref="A509:J509"/>
     <mergeCell ref="A5:J5"/>
@@ -16535,12 +16541,6 @@
     <mergeCell ref="A505:J505"/>
     <mergeCell ref="A506:J506"/>
     <mergeCell ref="A507:J507"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>